<commit_message>
Update pengajuan hbs pakai
</commit_message>
<xml_diff>
--- a/Tugas/Tanggal 18/Pak Munadi/1. Pengajuan Bahan Habis Pakai.xlsx
+++ b/Tugas/Tanggal 18/Pak Munadi/1. Pengajuan Bahan Habis Pakai.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DWI KURNIAWAN\Magang-Undip\Materi\18 Oktober\2021_PLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DWI KURNIAWAN\Magang-Undip\Tugas\Tanggal 18\Pak Munadi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23295" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bahan Habis Pakai" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Lab. ….........</t>
   </si>
   <si>
-    <t>Lab. Proses Produksi dan CNC</t>
-  </si>
-  <si>
     <t xml:space="preserve">RAM HP PC4-19200 ECC UDIMM DDR4 8GB 2400Mhz </t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>https://www.tokopedia.com/sanjayacomtronix/belden-ap700008-konektor-rj45-connector-rj45-cat-6?src=topads</t>
+  </si>
+  <si>
+    <t>Lab. Jurusan Teknik Elektro</t>
   </si>
 </sst>
 </file>
@@ -575,134 +575,134 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1043,32 +1043,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
     </row>
     <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -1434,61 +1434,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="70" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="82" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="69" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="81" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="74" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="73" customWidth="1"/>
     <col min="11" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="6" spans="1:10" s="42" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="78" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="25" t="s">
@@ -1514,428 +1514,428 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="80"/>
+      <c r="A7" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="35"/>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="32"/>
       <c r="I7" s="32"/>
-      <c r="J7" s="71"/>
+      <c r="J7" s="70"/>
     </row>
     <row r="8" spans="1:10" s="42" customFormat="1" ht="112.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="A8" s="51">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="51">
+        <v>22</v>
+      </c>
+      <c r="G8" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="52">
-        <v>22</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="54">
+      <c r="H8" s="53">
         <f>1850000*110%</f>
         <v>2035000.0000000002</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="53">
         <f>F8*H8</f>
         <v>44770000.000000007</v>
       </c>
-      <c r="J8" s="55" t="s">
-        <v>18</v>
+      <c r="J8" s="54" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="59">
+      <c r="A9" s="58">
         <v>2</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="F9" s="58">
+        <v>4</v>
+      </c>
+      <c r="G9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="59">
-        <v>4</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="60">
+      <c r="H9" s="59">
         <f>474088*110%</f>
         <v>521496.80000000005</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="53">
         <f>F9*H9</f>
         <v>2085987.2000000002</v>
       </c>
-      <c r="J9" s="72" t="s">
+      <c r="J9" s="71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>3</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="58" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
-        <v>3</v>
-      </c>
-      <c r="B10" s="78" t="s">
+      <c r="F10" s="58">
         <v>30</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="59">
-        <v>30</v>
-      </c>
-      <c r="G10" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="60">
+      <c r="G10" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="59">
         <f>40000*110%</f>
         <v>44000</v>
       </c>
-      <c r="I10" s="54">
+      <c r="I10" s="53">
         <f>F10*H10</f>
         <v>1320000</v>
       </c>
-      <c r="J10" s="72" t="s">
-        <v>29</v>
+      <c r="J10" s="71" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="57" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
+      <c r="A11" s="58">
         <v>4</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="D11" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="E11" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="59">
+      <c r="F11" s="58">
         <v>1</v>
       </c>
-      <c r="G11" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="60">
+      <c r="G11" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="59">
         <f>1900000*110%</f>
         <v>2090000.0000000002</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="53">
         <f>F11*H11</f>
         <v>2090000.0000000002</v>
       </c>
-      <c r="J11" s="72" t="s">
+      <c r="J11" s="71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="58">
+        <v>5</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="82" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="59">
-        <v>5</v>
-      </c>
-      <c r="B12" s="61" t="s">
+      <c r="D12" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="58">
+        <v>1</v>
+      </c>
+      <c r="G12" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="59">
-        <v>1</v>
-      </c>
-      <c r="G12" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="60">
+      <c r="H12" s="59">
         <f>400000*110%</f>
         <v>440000.00000000006</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I12" s="53">
         <f>F12*H12</f>
         <v>440000.00000000006</v>
       </c>
-      <c r="J12" s="72" t="s">
-        <v>39</v>
+      <c r="J12" s="71" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="81"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="80"/>
       <c r="D32" s="8"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="73">
+      <c r="J32" s="72">
         <v>0</v>
       </c>
     </row>

</xml_diff>